<commit_message>
setting up the paper trading file to initialise with the last 3 months of data from the table for now.
</commit_message>
<xml_diff>
--- a/banks to trade on.xlsx
+++ b/banks to trade on.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/04919e902f25d8eb/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B4211F8-322A-48F5-982C-D4B3798B4312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{8B4211F8-322A-48F5-982C-D4B3798B4312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2433D78-92C9-48ED-9CA2-723675FF141A}"/>
   <bookViews>
     <workbookView xWindow="-12405" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{75870254-B14B-4C82-9F15-A5454906F955}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>HDB</t>
   </si>
@@ -337,6 +337,9 @@
   </si>
   <si>
     <t>BCS</t>
+  </si>
+  <si>
+    <t>Banks</t>
   </si>
 </sst>
 </file>
@@ -756,616 +759,621 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41859714-CB06-4F2E-B402-1721E165D3E6}">
-  <dimension ref="A1:A100"/>
+  <dimension ref="A1:A101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+    <row r="23" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
+    <row r="31" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
+    <row r="35" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
+    <row r="37" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
+    <row r="39" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
+    <row r="41" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
+    <row r="43" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
+    <row r="47" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
+    <row r="48" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="2" t="s">
+    <row r="49" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="2" t="s">
+    <row r="51" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="2" t="s">
+    <row r="53" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="2" t="s">
+    <row r="55" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="2" t="s">
+    <row r="57" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="2" t="s">
+    <row r="59" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="2" t="s">
+    <row r="61" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="2" t="s">
+    <row r="63" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="2" t="s">
+    <row r="65" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="2" t="s">
+    <row r="67" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="2" t="s">
+    <row r="69" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="2" t="s">
+    <row r="71" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="2" t="s">
+    <row r="73" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="2" t="s">
+    <row r="75" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="1" t="s">
+    <row r="76" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="2" t="s">
+    <row r="77" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="2" t="s">
+    <row r="79" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="2" t="s">
+    <row r="81" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="2" t="s">
+    <row r="83" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="2" t="s">
+    <row r="85" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="1" t="s">
+    <row r="86" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="2" t="s">
+    <row r="87" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="1" t="s">
+    <row r="88" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="2" t="s">
+    <row r="89" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="1" t="s">
+    <row r="90" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="2" t="s">
+    <row r="91" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="2" t="s">
+    <row r="93" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="1" t="s">
+    <row r="94" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="2" t="s">
+    <row r="95" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="1" t="s">
+    <row r="96" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="2" t="s">
+    <row r="97" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="1" t="s">
+    <row r="98" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="2" t="s">
+    <row r="99" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="1" t="s">
+    <row r="100" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="3" t="s">
+    <row r="101" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="3" t="s">
         <v>79</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://stockanalysis.com/stocks/jpm/" xr:uid="{F4464F62-8663-4C87-AD79-4BB3FD24A957}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://stockanalysis.com/stocks/bac/" xr:uid="{A7773DEC-B211-41BA-8135-ADA47543D9DF}"/>
-    <hyperlink ref="A3" r:id="rId3" display="https://stockanalysis.com/stocks/wfc/" xr:uid="{2645D11A-9B2F-432C-8FE5-66BA9D9F130F}"/>
-    <hyperlink ref="A4" r:id="rId4" display="https://stockanalysis.com/stocks/hsbc/" xr:uid="{BC69509D-4790-4145-B2FA-263999EF39E3}"/>
-    <hyperlink ref="A5" r:id="rId5" display="https://stockanalysis.com/stocks/ry/" xr:uid="{C28F15FC-EDAF-42D1-83C6-915D8C71F90B}"/>
-    <hyperlink ref="A6" r:id="rId6" display="https://stockanalysis.com/stocks/hdb/" xr:uid="{30B5C12A-A8E0-41E1-942A-19766203A62D}"/>
-    <hyperlink ref="A7" r:id="rId7" display="https://stockanalysis.com/stocks/c/" xr:uid="{BDAA848F-186A-495D-8B6C-70EAFA5F71EC}"/>
-    <hyperlink ref="A8" r:id="rId8" display="https://stockanalysis.com/stocks/mufg/" xr:uid="{812C5790-65BC-4161-983C-56EBD8E91D20}"/>
-    <hyperlink ref="A9" r:id="rId9" display="https://stockanalysis.com/stocks/td/" xr:uid="{A928CC99-FF34-41FF-93E5-1535F42C7AFC}"/>
-    <hyperlink ref="A10" r:id="rId10" display="https://stockanalysis.com/stocks/san/" xr:uid="{FDC249F3-D43B-44A6-AEBE-2FE3413A6228}"/>
-    <hyperlink ref="A11" r:id="rId11" display="https://stockanalysis.com/stocks/ibn/" xr:uid="{A7FB18D9-935B-4053-A4DF-A0117C16EE79}"/>
-    <hyperlink ref="A12" r:id="rId12" display="https://stockanalysis.com/stocks/ubs/" xr:uid="{0F5AC41A-3C76-4206-B214-27B5F7B01A3A}"/>
-    <hyperlink ref="A13" r:id="rId13" display="https://stockanalysis.com/stocks/smfg/" xr:uid="{15CB66DE-DEE4-4493-A5B9-E248F96A3686}"/>
-    <hyperlink ref="A14" r:id="rId14" display="https://stockanalysis.com/stocks/bbva/" xr:uid="{E7B1828D-FA7B-47EA-9DD9-C618A4477A2C}"/>
-    <hyperlink ref="A15" r:id="rId15" display="https://stockanalysis.com/stocks/bmo/" xr:uid="{98B5785C-3367-45BB-BC2D-6E63B39D497C}"/>
-    <hyperlink ref="A16" r:id="rId16" display="https://stockanalysis.com/stocks/pnc/" xr:uid="{879A3C35-BFE2-492B-AD0B-756E5C6157D9}"/>
-    <hyperlink ref="A17" r:id="rId17" display="https://stockanalysis.com/stocks/usb/" xr:uid="{40978D3F-C782-4D4A-928A-87B50E3C82D1}"/>
-    <hyperlink ref="A18" r:id="rId18" display="https://stockanalysis.com/stocks/bk/" xr:uid="{4FA9BDC8-0570-434B-8129-E466649228DE}"/>
-    <hyperlink ref="A19" r:id="rId19" display="https://stockanalysis.com/stocks/mfg/" xr:uid="{8DC7B36C-44F0-4B00-A93C-C257107053BB}"/>
-    <hyperlink ref="A20" r:id="rId20" display="https://stockanalysis.com/stocks/bns/" xr:uid="{777718CF-15C1-4ADB-8815-BC08D3FFA697}"/>
-    <hyperlink ref="A21" r:id="rId21" display="https://stockanalysis.com/stocks/cm/" xr:uid="{70A18432-7D1C-44B3-AAEA-8654D2B60041}"/>
-    <hyperlink ref="A22" r:id="rId22" display="https://stockanalysis.com/stocks/ing/" xr:uid="{9835521E-77EF-4F58-82EC-54BD96D3DCE0}"/>
-    <hyperlink ref="A23" r:id="rId23" display="https://stockanalysis.com/stocks/bcs/" xr:uid="{72245BF7-9E86-4E1D-9BAA-06BEFEECEEC2}"/>
-    <hyperlink ref="A24" r:id="rId24" display="https://stockanalysis.com/stocks/itub/" xr:uid="{C0F98AC9-6218-4E96-854C-327F67882E5D}"/>
-    <hyperlink ref="A25" r:id="rId25" display="https://stockanalysis.com/stocks/nu/" xr:uid="{ED31179F-32A4-4C7F-ACEC-532DBAD7F8CC}"/>
-    <hyperlink ref="A26" r:id="rId26" display="https://stockanalysis.com/stocks/lyg/" xr:uid="{FDDA9C5C-6438-4340-BB37-154F0C5B8E88}"/>
-    <hyperlink ref="A27" r:id="rId27" display="https://stockanalysis.com/stocks/db/" xr:uid="{0C3346F5-210A-4A6B-9A2E-71BB7161F9B0}"/>
-    <hyperlink ref="A28" r:id="rId28" display="https://stockanalysis.com/stocks/tfc/" xr:uid="{CC678C45-0061-4D6B-8B73-E3BAEA2D6703}"/>
-    <hyperlink ref="A29" r:id="rId29" display="https://stockanalysis.com/stocks/nwg/" xr:uid="{DB76E24D-B89F-4603-B5E6-2376F37A4DC4}"/>
-    <hyperlink ref="A30" r:id="rId30" display="https://stockanalysis.com/stocks/mtb/" xr:uid="{104149EC-9D57-4F3B-A50E-36A4B30B1F97}"/>
-    <hyperlink ref="A31" r:id="rId31" display="https://stockanalysis.com/stocks/kb/" xr:uid="{A1421CF0-25E3-4D70-86DF-34B5C36B5EB6}"/>
-    <hyperlink ref="A32" r:id="rId32" display="https://stockanalysis.com/stocks/fitb/" xr:uid="{349847CC-E8CD-495D-B5CB-1EBA511A609A}"/>
-    <hyperlink ref="A33" r:id="rId33" display="https://stockanalysis.com/stocks/fcnca/" xr:uid="{EEB965DA-C0B4-47D2-B472-F76DF2BB65A0}"/>
-    <hyperlink ref="A34" r:id="rId34" display="https://stockanalysis.com/stocks/bbd/" xr:uid="{F43FBEFA-5F18-4041-98D6-0F877108C4C7}"/>
-    <hyperlink ref="A35" r:id="rId35" display="https://stockanalysis.com/stocks/hban/" xr:uid="{2A111D6F-BCFD-4D28-8B0F-A1ABE88F0FE7}"/>
-    <hyperlink ref="A36" r:id="rId36" display="https://stockanalysis.com/stocks/shg/" xr:uid="{B813067D-A939-4B9F-BC17-02622CDF4CDC}"/>
-    <hyperlink ref="A37" r:id="rId37" display="https://stockanalysis.com/stocks/rf/" xr:uid="{94097CAF-E5C2-4248-9A91-C5BEADDF6818}"/>
-    <hyperlink ref="A38" r:id="rId38" display="https://stockanalysis.com/stocks/cfg/" xr:uid="{46D76859-69FE-4A00-AD5A-517E9BF2A5CE}"/>
-    <hyperlink ref="A39" r:id="rId39" display="https://stockanalysis.com/stocks/key/" xr:uid="{AF3BA3DD-E26A-4E04-ACBB-252021866DCB}"/>
-    <hyperlink ref="A40" r:id="rId40" display="https://stockanalysis.com/stocks/bap/" xr:uid="{F41D8E5A-34FC-4D55-8EBD-E12351CB3A96}"/>
-    <hyperlink ref="A41" r:id="rId41" display="https://stockanalysis.com/stocks/bsbr/" xr:uid="{B135ACDD-60A3-45B4-8E94-A70CCC5E4BAB}"/>
-    <hyperlink ref="A42" r:id="rId42" display="https://stockanalysis.com/stocks/ewbc/" xr:uid="{21B34E71-99F9-4CDE-83E6-AA7CA21A7793}"/>
-    <hyperlink ref="A43" r:id="rId43" display="https://stockanalysis.com/stocks/bch/" xr:uid="{0DFEA0F0-0618-48DB-8055-209498F085D0}"/>
-    <hyperlink ref="A44" r:id="rId44" display="https://stockanalysis.com/stocks/wf/" xr:uid="{7FC705A1-1F00-476E-8F53-5C23B8733B80}"/>
-    <hyperlink ref="A45" r:id="rId45" display="https://stockanalysis.com/stocks/cib/" xr:uid="{E3AFCC68-F735-4E56-83CD-48D953B8296E}"/>
-    <hyperlink ref="A46" r:id="rId46" display="https://stockanalysis.com/stocks/chym/" xr:uid="{D7960B2E-247C-4939-8CB3-8D85AE25A67F}"/>
-    <hyperlink ref="A47" r:id="rId47" display="https://stockanalysis.com/stocks/bsac/" xr:uid="{035CFF45-05BE-4BF7-A327-5152A8C9BBE1}"/>
-    <hyperlink ref="A48" r:id="rId48" display="https://stockanalysis.com/stocks/fhn/" xr:uid="{82FC5665-D823-4240-BF3A-E3B413D0A103}"/>
-    <hyperlink ref="A49" r:id="rId49" display="https://stockanalysis.com/stocks/wbs/" xr:uid="{C0397E95-B4D4-4DB9-A0D9-3E7A3F630E63}"/>
-    <hyperlink ref="A50" r:id="rId50" display="https://stockanalysis.com/stocks/ssb/" xr:uid="{2DEF83CD-062B-4CC8-9AFF-54760901EF11}"/>
-    <hyperlink ref="A51" r:id="rId51" display="https://stockanalysis.com/stocks/pnfp/" xr:uid="{62F35FB0-AE34-44D3-A062-97447C47E09B}"/>
-    <hyperlink ref="A52" r:id="rId52" display="https://stockanalysis.com/stocks/wtfc/" xr:uid="{5CD163D6-1B73-45FF-95EE-CB4930DA236A}"/>
-    <hyperlink ref="A53" r:id="rId53" display="https://stockanalysis.com/stocks/cfr/" xr:uid="{F414BE22-2620-4372-8815-D65597FDB4FA}"/>
-    <hyperlink ref="A54" r:id="rId54" display="https://stockanalysis.com/stocks/wal/" xr:uid="{FA4D140F-B1C9-4824-B8B2-EADE21D6557B}"/>
-    <hyperlink ref="A55" r:id="rId55" display="https://stockanalysis.com/stocks/cbsh/" xr:uid="{6E876CAF-009E-4DA2-92F4-D4216B6C8FA7}"/>
-    <hyperlink ref="A56" r:id="rId56" display="https://stockanalysis.com/stocks/cma/" xr:uid="{984C0347-C6EA-4E22-9B34-BBAD0138FE0E}"/>
-    <hyperlink ref="A57" r:id="rId57" display="https://stockanalysis.com/stocks/onb/" xr:uid="{04914F96-1CD4-4900-952D-D1C31E7E6DBC}"/>
-    <hyperlink ref="A58" r:id="rId58" display="https://stockanalysis.com/stocks/zion/" xr:uid="{FBD6123D-7BBA-445A-BC8C-7B8EC943334D}"/>
-    <hyperlink ref="A59" r:id="rId59" display="https://stockanalysis.com/stocks/umbf/" xr:uid="{C273339E-B134-48CC-B842-128F7652EFBB}"/>
-    <hyperlink ref="A60" r:id="rId60" display="https://stockanalysis.com/stocks/bpop/" xr:uid="{ADC0A4CB-8A39-4089-BBEB-4CE09AE68522}"/>
-    <hyperlink ref="A61" r:id="rId61" display="https://stockanalysis.com/stocks/snv/" xr:uid="{62620493-A1BC-4276-8674-1DA35987B1AB}"/>
-    <hyperlink ref="A62" r:id="rId62" display="https://stockanalysis.com/stocks/ggal/" xr:uid="{C9B8CF0B-8F04-4E69-A4ED-EAE242D4EA55}"/>
-    <hyperlink ref="A63" r:id="rId63" display="https://stockanalysis.com/stocks/pb/" xr:uid="{17595FA2-5C37-420A-9304-A631E8494808}"/>
-    <hyperlink ref="A64" r:id="rId64" display="https://stockanalysis.com/stocks/bokf/" xr:uid="{B03F91EE-A90D-4C94-A8F7-3CCCDAA68FCD}"/>
-    <hyperlink ref="A65" r:id="rId65" display="https://stockanalysis.com/stocks/cade/" xr:uid="{758C3545-AA7B-4823-B2C8-9B3E3F6D2F3A}"/>
-    <hyperlink ref="A66" r:id="rId66" display="https://stockanalysis.com/stocks/homb/" xr:uid="{E8D9AD06-800F-4800-9608-D123D852B8D5}"/>
-    <hyperlink ref="A67" r:id="rId67" display="https://stockanalysis.com/stocks/ozk/" xr:uid="{D8CFA97F-8D23-4CF4-9F21-3A933DD9F109}"/>
-    <hyperlink ref="A68" r:id="rId68" display="https://stockanalysis.com/stocks/fnb/" xr:uid="{663DC536-C8DB-4C06-8E11-BD06B86F6E53}"/>
-    <hyperlink ref="A69" r:id="rId69" display="https://stockanalysis.com/stocks/gbci/" xr:uid="{F81DD899-9AF0-43BA-8E9D-D7CD8229F7B9}"/>
-    <hyperlink ref="A70" r:id="rId70" display="https://stockanalysis.com/stocks/vly/" xr:uid="{B2F8A56B-0350-4016-9281-DF2A433431AE}"/>
-    <hyperlink ref="A71" r:id="rId71" display="https://stockanalysis.com/stocks/ffin/" xr:uid="{951C886B-2B76-4A05-8489-FB51A5FA0896}"/>
-    <hyperlink ref="A72" r:id="rId72" display="https://stockanalysis.com/stocks/ubsi/" xr:uid="{24338C5B-CD43-45BF-BBC8-2F0ECB47C932}"/>
-    <hyperlink ref="A73" r:id="rId73" display="https://stockanalysis.com/stocks/hwc/" xr:uid="{388A8EF5-FA7D-45F2-BBDE-435821B73853}"/>
-    <hyperlink ref="A74" r:id="rId74" display="https://stockanalysis.com/stocks/colb/" xr:uid="{DF4B8605-B285-4A2D-B8C8-01F0C6289EEF}"/>
-    <hyperlink ref="A75" r:id="rId75" display="https://stockanalysis.com/stocks/flg/" xr:uid="{C540C5F3-1CD6-402B-A6CA-3D6AA7590D9D}"/>
-    <hyperlink ref="A76" r:id="rId76" display="https://stockanalysis.com/stocks/ax/" xr:uid="{36409166-46ED-41B2-A313-396CCC63EFF4}"/>
-    <hyperlink ref="A77" r:id="rId77" display="https://stockanalysis.com/stocks/aub/" xr:uid="{D4A55D52-7306-4C5E-8C12-21317F8981CB}"/>
-    <hyperlink ref="A78" r:id="rId78" display="https://stockanalysis.com/stocks/abcb/" xr:uid="{B1891343-60B2-4824-B9C6-A3E0FAF8268F}"/>
-    <hyperlink ref="A79" r:id="rId79" display="https://stockanalysis.com/stocks/sfbs/" xr:uid="{69090A66-2A9C-4078-B1B4-913FA75EB530}"/>
-    <hyperlink ref="A80" r:id="rId80" display="https://stockanalysis.com/stocks/banf/" xr:uid="{45221A68-ECB9-431B-BC64-C613D644FB5E}"/>
-    <hyperlink ref="A81" r:id="rId81" display="https://stockanalysis.com/stocks/iboc/" xr:uid="{482118DC-40A5-40FA-A200-6FF055AAF1B9}"/>
-    <hyperlink ref="A82" r:id="rId82" display="https://stockanalysis.com/stocks/asb/" xr:uid="{66AA2ED6-8B3F-4394-8B4C-0492A75AF15E}"/>
-    <hyperlink ref="A83" r:id="rId83" display="https://stockanalysis.com/stocks/ifs/" xr:uid="{43211E34-A96C-4440-8CBB-3C0B65508C4A}"/>
-    <hyperlink ref="A84" r:id="rId84" display="https://stockanalysis.com/stocks/bma/" xr:uid="{5B31AFE4-0F65-48F2-B85B-1FC504A64EF2}"/>
-    <hyperlink ref="A85" r:id="rId85" display="https://stockanalysis.com/stocks/tcbi/" xr:uid="{13331413-0BFB-4B42-9B32-C3671E7F6346}"/>
-    <hyperlink ref="A86" r:id="rId86" display="https://stockanalysis.com/stocks/ucb/" xr:uid="{7E9993FA-E015-425F-9EB3-8516BE1424B9}"/>
-    <hyperlink ref="A87" r:id="rId87" display="https://stockanalysis.com/stocks/rnst/" xr:uid="{E1B8BAA8-207B-4658-A07E-E37D1F59F9C5}"/>
-    <hyperlink ref="A88" r:id="rId88" display="https://stockanalysis.com/stocks/tfsl/" xr:uid="{97A65834-B9D6-49BD-9244-C4ED94BEB3F5}"/>
-    <hyperlink ref="A89" r:id="rId89" display="https://stockanalysis.com/stocks/fult/" xr:uid="{843999A5-3650-436A-A2AE-72993026F93F}"/>
-    <hyperlink ref="A90" r:id="rId90" display="https://stockanalysis.com/stocks/fbp/" xr:uid="{84A78E5F-334B-42D9-BAD3-BAE7EE3C7A63}"/>
-    <hyperlink ref="A91" r:id="rId91" display="https://stockanalysis.com/stocks/indb/" xr:uid="{722F1A23-39BA-4082-BCE8-1AD8732872EF}"/>
-    <hyperlink ref="A92" r:id="rId92" display="https://stockanalysis.com/stocks/aval/" xr:uid="{77263147-A7B2-4F34-B056-126CA6142F4A}"/>
-    <hyperlink ref="A93" r:id="rId93" display="https://stockanalysis.com/stocks/caty/" xr:uid="{F7D306D9-2722-4307-A0CA-8FDB090A092B}"/>
-    <hyperlink ref="A94" r:id="rId94" display="https://stockanalysis.com/stocks/wsfs/" xr:uid="{0B8BBBB5-A5B1-47C1-B1EE-93B8DB9D1943}"/>
-    <hyperlink ref="A95" r:id="rId95" display="https://stockanalysis.com/stocks/fibk/" xr:uid="{72EA2A13-766E-4284-B6FA-6411E8E1F7F8}"/>
-    <hyperlink ref="A96" r:id="rId96" display="https://stockanalysis.com/stocks/fhb/" xr:uid="{E76B0200-9A2A-4953-A8B7-F43A9E917B25}"/>
-    <hyperlink ref="A97" r:id="rId97" display="https://stockanalysis.com/stocks/ebc/" xr:uid="{E1132BF1-55D5-4276-9B93-2DEFA80D3DEE}"/>
-    <hyperlink ref="A98" r:id="rId98" display="https://stockanalysis.com/stocks/tbbk/" xr:uid="{8866BD53-FC8B-4EDF-98C6-67F42E5E1609}"/>
-    <hyperlink ref="A99" r:id="rId99" display="https://stockanalysis.com/stocks/intr/" xr:uid="{69D23C9A-D249-43DE-8E5D-192462B56846}"/>
-    <hyperlink ref="A100" r:id="rId100" display="https://stockanalysis.com/stocks/wsbc/" xr:uid="{8EE56EFB-4102-4FB5-8577-175BB69B13D8}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://stockanalysis.com/stocks/jpm/" xr:uid="{F4464F62-8663-4C87-AD79-4BB3FD24A957}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://stockanalysis.com/stocks/bac/" xr:uid="{A7773DEC-B211-41BA-8135-ADA47543D9DF}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://stockanalysis.com/stocks/wfc/" xr:uid="{2645D11A-9B2F-432C-8FE5-66BA9D9F130F}"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://stockanalysis.com/stocks/hsbc/" xr:uid="{BC69509D-4790-4145-B2FA-263999EF39E3}"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://stockanalysis.com/stocks/ry/" xr:uid="{C28F15FC-EDAF-42D1-83C6-915D8C71F90B}"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://stockanalysis.com/stocks/hdb/" xr:uid="{30B5C12A-A8E0-41E1-942A-19766203A62D}"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://stockanalysis.com/stocks/c/" xr:uid="{BDAA848F-186A-495D-8B6C-70EAFA5F71EC}"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://stockanalysis.com/stocks/mufg/" xr:uid="{812C5790-65BC-4161-983C-56EBD8E91D20}"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://stockanalysis.com/stocks/td/" xr:uid="{A928CC99-FF34-41FF-93E5-1535F42C7AFC}"/>
+    <hyperlink ref="A11" r:id="rId10" display="https://stockanalysis.com/stocks/san/" xr:uid="{FDC249F3-D43B-44A6-AEBE-2FE3413A6228}"/>
+    <hyperlink ref="A12" r:id="rId11" display="https://stockanalysis.com/stocks/ibn/" xr:uid="{A7FB18D9-935B-4053-A4DF-A0117C16EE79}"/>
+    <hyperlink ref="A13" r:id="rId12" display="https://stockanalysis.com/stocks/ubs/" xr:uid="{0F5AC41A-3C76-4206-B214-27B5F7B01A3A}"/>
+    <hyperlink ref="A14" r:id="rId13" display="https://stockanalysis.com/stocks/smfg/" xr:uid="{15CB66DE-DEE4-4493-A5B9-E248F96A3686}"/>
+    <hyperlink ref="A15" r:id="rId14" display="https://stockanalysis.com/stocks/bbva/" xr:uid="{E7B1828D-FA7B-47EA-9DD9-C618A4477A2C}"/>
+    <hyperlink ref="A16" r:id="rId15" display="https://stockanalysis.com/stocks/bmo/" xr:uid="{98B5785C-3367-45BB-BC2D-6E63B39D497C}"/>
+    <hyperlink ref="A17" r:id="rId16" display="https://stockanalysis.com/stocks/pnc/" xr:uid="{879A3C35-BFE2-492B-AD0B-756E5C6157D9}"/>
+    <hyperlink ref="A18" r:id="rId17" display="https://stockanalysis.com/stocks/usb/" xr:uid="{40978D3F-C782-4D4A-928A-87B50E3C82D1}"/>
+    <hyperlink ref="A19" r:id="rId18" display="https://stockanalysis.com/stocks/bk/" xr:uid="{4FA9BDC8-0570-434B-8129-E466649228DE}"/>
+    <hyperlink ref="A20" r:id="rId19" display="https://stockanalysis.com/stocks/mfg/" xr:uid="{8DC7B36C-44F0-4B00-A93C-C257107053BB}"/>
+    <hyperlink ref="A21" r:id="rId20" display="https://stockanalysis.com/stocks/bns/" xr:uid="{777718CF-15C1-4ADB-8815-BC08D3FFA697}"/>
+    <hyperlink ref="A22" r:id="rId21" display="https://stockanalysis.com/stocks/cm/" xr:uid="{70A18432-7D1C-44B3-AAEA-8654D2B60041}"/>
+    <hyperlink ref="A23" r:id="rId22" display="https://stockanalysis.com/stocks/ing/" xr:uid="{9835521E-77EF-4F58-82EC-54BD96D3DCE0}"/>
+    <hyperlink ref="A24" r:id="rId23" display="https://stockanalysis.com/stocks/bcs/" xr:uid="{72245BF7-9E86-4E1D-9BAA-06BEFEECEEC2}"/>
+    <hyperlink ref="A25" r:id="rId24" display="https://stockanalysis.com/stocks/itub/" xr:uid="{C0F98AC9-6218-4E96-854C-327F67882E5D}"/>
+    <hyperlink ref="A26" r:id="rId25" display="https://stockanalysis.com/stocks/nu/" xr:uid="{ED31179F-32A4-4C7F-ACEC-532DBAD7F8CC}"/>
+    <hyperlink ref="A27" r:id="rId26" display="https://stockanalysis.com/stocks/lyg/" xr:uid="{FDDA9C5C-6438-4340-BB37-154F0C5B8E88}"/>
+    <hyperlink ref="A28" r:id="rId27" display="https://stockanalysis.com/stocks/db/" xr:uid="{0C3346F5-210A-4A6B-9A2E-71BB7161F9B0}"/>
+    <hyperlink ref="A29" r:id="rId28" display="https://stockanalysis.com/stocks/tfc/" xr:uid="{CC678C45-0061-4D6B-8B73-E3BAEA2D6703}"/>
+    <hyperlink ref="A30" r:id="rId29" display="https://stockanalysis.com/stocks/nwg/" xr:uid="{DB76E24D-B89F-4603-B5E6-2376F37A4DC4}"/>
+    <hyperlink ref="A31" r:id="rId30" display="https://stockanalysis.com/stocks/mtb/" xr:uid="{104149EC-9D57-4F3B-A50E-36A4B30B1F97}"/>
+    <hyperlink ref="A32" r:id="rId31" display="https://stockanalysis.com/stocks/kb/" xr:uid="{A1421CF0-25E3-4D70-86DF-34B5C36B5EB6}"/>
+    <hyperlink ref="A33" r:id="rId32" display="https://stockanalysis.com/stocks/fitb/" xr:uid="{349847CC-E8CD-495D-B5CB-1EBA511A609A}"/>
+    <hyperlink ref="A34" r:id="rId33" display="https://stockanalysis.com/stocks/fcnca/" xr:uid="{EEB965DA-C0B4-47D2-B472-F76DF2BB65A0}"/>
+    <hyperlink ref="A35" r:id="rId34" display="https://stockanalysis.com/stocks/bbd/" xr:uid="{F43FBEFA-5F18-4041-98D6-0F877108C4C7}"/>
+    <hyperlink ref="A36" r:id="rId35" display="https://stockanalysis.com/stocks/hban/" xr:uid="{2A111D6F-BCFD-4D28-8B0F-A1ABE88F0FE7}"/>
+    <hyperlink ref="A37" r:id="rId36" display="https://stockanalysis.com/stocks/shg/" xr:uid="{B813067D-A939-4B9F-BC17-02622CDF4CDC}"/>
+    <hyperlink ref="A38" r:id="rId37" display="https://stockanalysis.com/stocks/rf/" xr:uid="{94097CAF-E5C2-4248-9A91-C5BEADDF6818}"/>
+    <hyperlink ref="A39" r:id="rId38" display="https://stockanalysis.com/stocks/cfg/" xr:uid="{46D76859-69FE-4A00-AD5A-517E9BF2A5CE}"/>
+    <hyperlink ref="A40" r:id="rId39" display="https://stockanalysis.com/stocks/key/" xr:uid="{AF3BA3DD-E26A-4E04-ACBB-252021866DCB}"/>
+    <hyperlink ref="A41" r:id="rId40" display="https://stockanalysis.com/stocks/bap/" xr:uid="{F41D8E5A-34FC-4D55-8EBD-E12351CB3A96}"/>
+    <hyperlink ref="A42" r:id="rId41" display="https://stockanalysis.com/stocks/bsbr/" xr:uid="{B135ACDD-60A3-45B4-8E94-A70CCC5E4BAB}"/>
+    <hyperlink ref="A43" r:id="rId42" display="https://stockanalysis.com/stocks/ewbc/" xr:uid="{21B34E71-99F9-4CDE-83E6-AA7CA21A7793}"/>
+    <hyperlink ref="A44" r:id="rId43" display="https://stockanalysis.com/stocks/bch/" xr:uid="{0DFEA0F0-0618-48DB-8055-209498F085D0}"/>
+    <hyperlink ref="A45" r:id="rId44" display="https://stockanalysis.com/stocks/wf/" xr:uid="{7FC705A1-1F00-476E-8F53-5C23B8733B80}"/>
+    <hyperlink ref="A46" r:id="rId45" display="https://stockanalysis.com/stocks/cib/" xr:uid="{E3AFCC68-F735-4E56-83CD-48D953B8296E}"/>
+    <hyperlink ref="A47" r:id="rId46" display="https://stockanalysis.com/stocks/chym/" xr:uid="{D7960B2E-247C-4939-8CB3-8D85AE25A67F}"/>
+    <hyperlink ref="A48" r:id="rId47" display="https://stockanalysis.com/stocks/bsac/" xr:uid="{035CFF45-05BE-4BF7-A327-5152A8C9BBE1}"/>
+    <hyperlink ref="A49" r:id="rId48" display="https://stockanalysis.com/stocks/fhn/" xr:uid="{82FC5665-D823-4240-BF3A-E3B413D0A103}"/>
+    <hyperlink ref="A50" r:id="rId49" display="https://stockanalysis.com/stocks/wbs/" xr:uid="{C0397E95-B4D4-4DB9-A0D9-3E7A3F630E63}"/>
+    <hyperlink ref="A51" r:id="rId50" display="https://stockanalysis.com/stocks/ssb/" xr:uid="{2DEF83CD-062B-4CC8-9AFF-54760901EF11}"/>
+    <hyperlink ref="A52" r:id="rId51" display="https://stockanalysis.com/stocks/pnfp/" xr:uid="{62F35FB0-AE34-44D3-A062-97447C47E09B}"/>
+    <hyperlink ref="A53" r:id="rId52" display="https://stockanalysis.com/stocks/wtfc/" xr:uid="{5CD163D6-1B73-45FF-95EE-CB4930DA236A}"/>
+    <hyperlink ref="A54" r:id="rId53" display="https://stockanalysis.com/stocks/cfr/" xr:uid="{F414BE22-2620-4372-8815-D65597FDB4FA}"/>
+    <hyperlink ref="A55" r:id="rId54" display="https://stockanalysis.com/stocks/wal/" xr:uid="{FA4D140F-B1C9-4824-B8B2-EADE21D6557B}"/>
+    <hyperlink ref="A56" r:id="rId55" display="https://stockanalysis.com/stocks/cbsh/" xr:uid="{6E876CAF-009E-4DA2-92F4-D4216B6C8FA7}"/>
+    <hyperlink ref="A57" r:id="rId56" display="https://stockanalysis.com/stocks/cma/" xr:uid="{984C0347-C6EA-4E22-9B34-BBAD0138FE0E}"/>
+    <hyperlink ref="A58" r:id="rId57" display="https://stockanalysis.com/stocks/onb/" xr:uid="{04914F96-1CD4-4900-952D-D1C31E7E6DBC}"/>
+    <hyperlink ref="A59" r:id="rId58" display="https://stockanalysis.com/stocks/zion/" xr:uid="{FBD6123D-7BBA-445A-BC8C-7B8EC943334D}"/>
+    <hyperlink ref="A60" r:id="rId59" display="https://stockanalysis.com/stocks/umbf/" xr:uid="{C273339E-B134-48CC-B842-128F7652EFBB}"/>
+    <hyperlink ref="A61" r:id="rId60" display="https://stockanalysis.com/stocks/bpop/" xr:uid="{ADC0A4CB-8A39-4089-BBEB-4CE09AE68522}"/>
+    <hyperlink ref="A62" r:id="rId61" display="https://stockanalysis.com/stocks/snv/" xr:uid="{62620493-A1BC-4276-8674-1DA35987B1AB}"/>
+    <hyperlink ref="A63" r:id="rId62" display="https://stockanalysis.com/stocks/ggal/" xr:uid="{C9B8CF0B-8F04-4E69-A4ED-EAE242D4EA55}"/>
+    <hyperlink ref="A64" r:id="rId63" display="https://stockanalysis.com/stocks/pb/" xr:uid="{17595FA2-5C37-420A-9304-A631E8494808}"/>
+    <hyperlink ref="A65" r:id="rId64" display="https://stockanalysis.com/stocks/bokf/" xr:uid="{B03F91EE-A90D-4C94-A8F7-3CCCDAA68FCD}"/>
+    <hyperlink ref="A66" r:id="rId65" display="https://stockanalysis.com/stocks/cade/" xr:uid="{758C3545-AA7B-4823-B2C8-9B3E3F6D2F3A}"/>
+    <hyperlink ref="A67" r:id="rId66" display="https://stockanalysis.com/stocks/homb/" xr:uid="{E8D9AD06-800F-4800-9608-D123D852B8D5}"/>
+    <hyperlink ref="A68" r:id="rId67" display="https://stockanalysis.com/stocks/ozk/" xr:uid="{D8CFA97F-8D23-4CF4-9F21-3A933DD9F109}"/>
+    <hyperlink ref="A69" r:id="rId68" display="https://stockanalysis.com/stocks/fnb/" xr:uid="{663DC536-C8DB-4C06-8E11-BD06B86F6E53}"/>
+    <hyperlink ref="A70" r:id="rId69" display="https://stockanalysis.com/stocks/gbci/" xr:uid="{F81DD899-9AF0-43BA-8E9D-D7CD8229F7B9}"/>
+    <hyperlink ref="A71" r:id="rId70" display="https://stockanalysis.com/stocks/vly/" xr:uid="{B2F8A56B-0350-4016-9281-DF2A433431AE}"/>
+    <hyperlink ref="A72" r:id="rId71" display="https://stockanalysis.com/stocks/ffin/" xr:uid="{951C886B-2B76-4A05-8489-FB51A5FA0896}"/>
+    <hyperlink ref="A73" r:id="rId72" display="https://stockanalysis.com/stocks/ubsi/" xr:uid="{24338C5B-CD43-45BF-BBC8-2F0ECB47C932}"/>
+    <hyperlink ref="A74" r:id="rId73" display="https://stockanalysis.com/stocks/hwc/" xr:uid="{388A8EF5-FA7D-45F2-BBDE-435821B73853}"/>
+    <hyperlink ref="A75" r:id="rId74" display="https://stockanalysis.com/stocks/colb/" xr:uid="{DF4B8605-B285-4A2D-B8C8-01F0C6289EEF}"/>
+    <hyperlink ref="A76" r:id="rId75" display="https://stockanalysis.com/stocks/flg/" xr:uid="{C540C5F3-1CD6-402B-A6CA-3D6AA7590D9D}"/>
+    <hyperlink ref="A77" r:id="rId76" display="https://stockanalysis.com/stocks/ax/" xr:uid="{36409166-46ED-41B2-A313-396CCC63EFF4}"/>
+    <hyperlink ref="A78" r:id="rId77" display="https://stockanalysis.com/stocks/aub/" xr:uid="{D4A55D52-7306-4C5E-8C12-21317F8981CB}"/>
+    <hyperlink ref="A79" r:id="rId78" display="https://stockanalysis.com/stocks/abcb/" xr:uid="{B1891343-60B2-4824-B9C6-A3E0FAF8268F}"/>
+    <hyperlink ref="A80" r:id="rId79" display="https://stockanalysis.com/stocks/sfbs/" xr:uid="{69090A66-2A9C-4078-B1B4-913FA75EB530}"/>
+    <hyperlink ref="A81" r:id="rId80" display="https://stockanalysis.com/stocks/banf/" xr:uid="{45221A68-ECB9-431B-BC64-C613D644FB5E}"/>
+    <hyperlink ref="A82" r:id="rId81" display="https://stockanalysis.com/stocks/iboc/" xr:uid="{482118DC-40A5-40FA-A200-6FF055AAF1B9}"/>
+    <hyperlink ref="A83" r:id="rId82" display="https://stockanalysis.com/stocks/asb/" xr:uid="{66AA2ED6-8B3F-4394-8B4C-0492A75AF15E}"/>
+    <hyperlink ref="A84" r:id="rId83" display="https://stockanalysis.com/stocks/ifs/" xr:uid="{43211E34-A96C-4440-8CBB-3C0B65508C4A}"/>
+    <hyperlink ref="A85" r:id="rId84" display="https://stockanalysis.com/stocks/bma/" xr:uid="{5B31AFE4-0F65-48F2-B85B-1FC504A64EF2}"/>
+    <hyperlink ref="A86" r:id="rId85" display="https://stockanalysis.com/stocks/tcbi/" xr:uid="{13331413-0BFB-4B42-9B32-C3671E7F6346}"/>
+    <hyperlink ref="A87" r:id="rId86" display="https://stockanalysis.com/stocks/ucb/" xr:uid="{7E9993FA-E015-425F-9EB3-8516BE1424B9}"/>
+    <hyperlink ref="A88" r:id="rId87" display="https://stockanalysis.com/stocks/rnst/" xr:uid="{E1B8BAA8-207B-4658-A07E-E37D1F59F9C5}"/>
+    <hyperlink ref="A89" r:id="rId88" display="https://stockanalysis.com/stocks/tfsl/" xr:uid="{97A65834-B9D6-49BD-9244-C4ED94BEB3F5}"/>
+    <hyperlink ref="A90" r:id="rId89" display="https://stockanalysis.com/stocks/fult/" xr:uid="{843999A5-3650-436A-A2AE-72993026F93F}"/>
+    <hyperlink ref="A91" r:id="rId90" display="https://stockanalysis.com/stocks/fbp/" xr:uid="{84A78E5F-334B-42D9-BAD3-BAE7EE3C7A63}"/>
+    <hyperlink ref="A92" r:id="rId91" display="https://stockanalysis.com/stocks/indb/" xr:uid="{722F1A23-39BA-4082-BCE8-1AD8732872EF}"/>
+    <hyperlink ref="A93" r:id="rId92" display="https://stockanalysis.com/stocks/aval/" xr:uid="{77263147-A7B2-4F34-B056-126CA6142F4A}"/>
+    <hyperlink ref="A94" r:id="rId93" display="https://stockanalysis.com/stocks/caty/" xr:uid="{F7D306D9-2722-4307-A0CA-8FDB090A092B}"/>
+    <hyperlink ref="A95" r:id="rId94" display="https://stockanalysis.com/stocks/wsfs/" xr:uid="{0B8BBBB5-A5B1-47C1-B1EE-93B8DB9D1943}"/>
+    <hyperlink ref="A96" r:id="rId95" display="https://stockanalysis.com/stocks/fibk/" xr:uid="{72EA2A13-766E-4284-B6FA-6411E8E1F7F8}"/>
+    <hyperlink ref="A97" r:id="rId96" display="https://stockanalysis.com/stocks/fhb/" xr:uid="{E76B0200-9A2A-4953-A8B7-F43A9E917B25}"/>
+    <hyperlink ref="A98" r:id="rId97" display="https://stockanalysis.com/stocks/ebc/" xr:uid="{E1132BF1-55D5-4276-9B93-2DEFA80D3DEE}"/>
+    <hyperlink ref="A99" r:id="rId98" display="https://stockanalysis.com/stocks/tbbk/" xr:uid="{8866BD53-FC8B-4EDF-98C6-67F42E5E1609}"/>
+    <hyperlink ref="A100" r:id="rId99" display="https://stockanalysis.com/stocks/intr/" xr:uid="{69D23C9A-D249-43DE-8E5D-192462B56846}"/>
+    <hyperlink ref="A101" r:id="rId100" display="https://stockanalysis.com/stocks/wsbc/" xr:uid="{8EE56EFB-4102-4FB5-8577-175BB69B13D8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId101"/>

</xml_diff>